<commit_message>
Lab03 - added TestLink file
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="164" documentId="8_{1400DE03-3D9F-45A4-BE32-F3417339F90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB4F74A-4018-4DA5-8978-6466115E6059}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{1400DE03-3D9F-45A4-BE32-F3417339F90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BC2A888-B10B-4AE7-85BB-60D46C3CC7BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -1354,9 +1354,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1369,7 +1366,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1393,83 +1405,89 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1477,8 +1495,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1489,59 +1540,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1890,8 +1890,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,12 +1904,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
       <c r="H1" s="32" t="s">
         <v>39</v>
       </c>
@@ -1917,11 +1917,11 @@
       <c r="J1" s="32"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="2"/>
@@ -2087,26 +2087,25 @@
     </row>
     <row r="26" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
+      <c r="B26" s="127"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="127"/>
+      <c r="J26" s="127"/>
+      <c r="K26" s="127"/>
+      <c r="L26" s="127"/>
+      <c r="M26" s="127"/>
+      <c r="N26" s="127"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B26:N26"/>
+  <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
@@ -2142,12 +2141,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H2" s="38"/>
@@ -2175,22 +2174,22 @@
       <c r="M4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="G5" s="72" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="G5" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
@@ -2205,36 +2204,36 @@
       <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="84" t="s">
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="84"/>
+      <c r="N6" s="86"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="69" t="s">
         <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="83"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="85"/>
       <c r="I7" s="9" t="s">
         <v>67</v>
       </c>
@@ -2247,16 +2246,16 @@
       <c r="L7" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="73" t="s">
+      <c r="M7" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="77"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>63</v>
@@ -2279,16 +2278,16 @@
       <c r="L8" s="8">
         <v>2</v>
       </c>
-      <c r="M8" s="80" t="s">
+      <c r="M8" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="81"/>
+      <c r="N8" s="83"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>3</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="69" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2313,16 +2312,16 @@
       <c r="L9" s="8">
         <v>2</v>
       </c>
-      <c r="M9" s="80" t="s">
+      <c r="M9" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="N9" s="81"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="2:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C10" s="85"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>65</v>
@@ -2343,16 +2342,16 @@
       <c r="L10" s="8">
         <v>-3</v>
       </c>
-      <c r="M10" s="86" t="s">
+      <c r="M10" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="N10" s="87"/>
+      <c r="N10" s="71"/>
     </row>
     <row r="11" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="69" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -2365,14 +2364,14 @@
       <c r="J11" s="46"/>
       <c r="K11" s="46"/>
       <c r="L11" s="45"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>6</v>
       </c>
-      <c r="C12" s="85"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>76</v>
@@ -2383,8 +2382,8 @@
       <c r="J12" s="46"/>
       <c r="K12" s="46"/>
       <c r="L12" s="45"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
@@ -2397,8 +2396,8 @@
       <c r="J13" s="46"/>
       <c r="K13" s="46"/>
       <c r="L13" s="45"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
@@ -2411,8 +2410,8 @@
       <c r="J14" s="46"/>
       <c r="K14" s="46"/>
       <c r="L14" s="45"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -2425,8 +2424,8 @@
       <c r="J15" s="46"/>
       <c r="K15" s="46"/>
       <c r="L15" s="45"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="70"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
@@ -2439,8 +2438,8 @@
       <c r="J16" s="46"/>
       <c r="K16" s="46"/>
       <c r="L16" s="45"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="72"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
@@ -2453,8 +2452,8 @@
       <c r="J17" s="49"/>
       <c r="K17" s="49"/>
       <c r="L17" s="48"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
@@ -2467,8 +2466,8 @@
       <c r="J18" s="49"/>
       <c r="K18" s="49"/>
       <c r="L18" s="48"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="74"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
@@ -2481,8 +2480,8 @@
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
@@ -2494,23 +2493,11 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="G5:N5"/>
@@ -2523,6 +2510,18 @@
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="M6:N6"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2537,7 +2536,7 @@
   <dimension ref="B1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,12 +2557,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="34" t="s">
@@ -2584,24 +2583,24 @@
       <c r="O3" s="36"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
     </row>
     <row r="6" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -2614,43 +2613,43 @@
         <v>12</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="75" t="s">
+      <c r="I6" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="90" t="s">
+      <c r="K6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="90" t="s">
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="93"/>
+      <c r="P6" s="97"/>
     </row>
     <row r="7" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="94">
+      <c r="B7" s="87">
         <v>1</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="91" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="83"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="85"/>
       <c r="K7" s="9" t="s">
         <v>67</v>
       </c>
@@ -2663,14 +2662,14 @@
       <c r="N7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="O7" s="73" t="s">
+      <c r="O7" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="77"/>
+      <c r="P7" s="81"/>
     </row>
     <row r="8" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
-      <c r="C8" s="99"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="52" t="s">
         <v>79</v>
       </c>
@@ -2696,14 +2695,14 @@
       <c r="N8" s="8">
         <v>2</v>
       </c>
-      <c r="O8" s="80" t="s">
+      <c r="O8" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="P8" s="81"/>
+      <c r="P8" s="83"/>
     </row>
     <row r="9" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95"/>
-      <c r="C9" s="99"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="53" t="s">
         <v>80</v>
       </c>
@@ -2727,16 +2726,16 @@
       <c r="N9" s="8">
         <v>2</v>
       </c>
-      <c r="O9" s="86" t="s">
+      <c r="O9" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="P9" s="87"/>
+      <c r="P9" s="71"/>
     </row>
     <row r="10" spans="2:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="94">
+      <c r="B10" s="87">
         <v>2</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="87" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -2762,14 +2761,14 @@
       <c r="N10" s="8">
         <v>2</v>
       </c>
-      <c r="O10" s="86" t="s">
+      <c r="O10" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="P10" s="87"/>
+      <c r="P10" s="71"/>
     </row>
     <row r="11" spans="2:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
-      <c r="C11" s="95"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="2" t="s">
         <v>82</v>
       </c>
@@ -2793,14 +2792,14 @@
       <c r="N11" s="8">
         <v>1</v>
       </c>
-      <c r="O11" s="80" t="s">
+      <c r="O11" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="83"/>
     </row>
     <row r="12" spans="2:16" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="2" t="s">
         <v>83</v>
       </c>
@@ -2824,14 +2823,14 @@
       <c r="N12" s="8">
         <v>0</v>
       </c>
-      <c r="O12" s="86" t="s">
+      <c r="O12" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="P12" s="87"/>
+      <c r="P12" s="71"/>
     </row>
     <row r="13" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="2" t="s">
         <v>84</v>
       </c>
@@ -2861,8 +2860,8 @@
       <c r="P13" s="44"/>
     </row>
     <row r="14" spans="2:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="2" t="s">
         <v>85</v>
       </c>
@@ -2892,8 +2891,8 @@
       <c r="P14" s="44"/>
     </row>
     <row r="15" spans="2:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
@@ -2925,10 +2924,10 @@
       <c r="P15" s="44"/>
     </row>
     <row r="16" spans="2:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="94">
+      <c r="B16" s="87">
         <v>3</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="87" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -2962,8 +2961,8 @@
       <c r="P16" s="44"/>
     </row>
     <row r="17" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="95"/>
-      <c r="C17" s="95"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
       <c r="D17" s="2" t="s">
         <v>89</v>
       </c>
@@ -2993,8 +2992,8 @@
       <c r="P17" s="44"/>
     </row>
     <row r="18" spans="2:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="2" t="s">
         <v>90</v>
       </c>
@@ -3018,10 +3017,10 @@
       <c r="N18" s="8">
         <v>2</v>
       </c>
-      <c r="O18" s="80" t="s">
+      <c r="O18" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="P18" s="81"/>
+      <c r="P18" s="83"/>
     </row>
     <row r="19" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="29"/>
@@ -3034,8 +3033,8 @@
       <c r="L19" s="56"/>
       <c r="M19" s="56"/>
       <c r="N19" s="56"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="29"/>
@@ -3048,8 +3047,8 @@
       <c r="L20" s="56"/>
       <c r="M20" s="56"/>
       <c r="N20" s="56"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
+      <c r="O20" s="98"/>
+      <c r="P20" s="98"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="29"/>
@@ -3062,8 +3061,8 @@
       <c r="L21" s="56"/>
       <c r="M21" s="56"/>
       <c r="N21" s="56"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="29"/>
@@ -3076,8 +3075,8 @@
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
+      <c r="O22" s="98"/>
+      <c r="P22" s="98"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="29"/>
@@ -3090,8 +3089,8 @@
       <c r="L23" s="56"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
+      <c r="O23" s="98"/>
+      <c r="P23" s="98"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="29"/>
@@ -3104,8 +3103,8 @@
       <c r="L24" s="56"/>
       <c r="M24" s="56"/>
       <c r="N24" s="56"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
+      <c r="O24" s="98"/>
+      <c r="P24" s="98"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="29"/>
@@ -3118,8 +3117,8 @@
       <c r="L25" s="56"/>
       <c r="M25" s="56"/>
       <c r="N25" s="56"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
+      <c r="O25" s="98"/>
+      <c r="P25" s="98"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="29"/>
@@ -3132,8 +3131,8 @@
       <c r="L26" s="56"/>
       <c r="M26" s="56"/>
       <c r="N26" s="56"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
+      <c r="O26" s="98"/>
+      <c r="P26" s="98"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="29"/>
@@ -3146,39 +3145,37 @@
       <c r="L27" s="56"/>
       <c r="M27" s="56"/>
       <c r="N27" s="56"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="98"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="92"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="96"/>
       <c r="N30" s="24"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="I31" s="89"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
-      <c r="M31" s="89"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
       <c r="N31" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
     <mergeCell ref="I31:M31"/>
     <mergeCell ref="G5:P5"/>
     <mergeCell ref="O7:P7"/>
@@ -3195,14 +3192,16 @@
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3217,8 +3216,8 @@
   </sheetPr>
   <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,56 +3233,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="84" t="s">
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="84"/>
+      <c r="K4" s="86"/>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="118"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="125"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="99"/>
       <c r="F5" s="11" t="s">
         <v>67</v>
       </c>
@@ -3307,7 +3306,7 @@
       <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="121" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -3340,7 +3339,7 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="116"/>
+      <c r="C7" s="121"/>
       <c r="D7" s="15" t="s">
         <v>101</v>
       </c>
@@ -3371,7 +3370,7 @@
         <f t="shared" ref="B8:B16" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="116"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="15" t="s">
         <v>103</v>
       </c>
@@ -3400,7 +3399,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="116"/>
+      <c r="C9" s="121"/>
       <c r="D9" s="15"/>
       <c r="E9" s="7" t="s">
         <v>105</v>
@@ -3429,7 +3428,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="116"/>
+      <c r="C10" s="121"/>
       <c r="D10" s="15"/>
       <c r="E10" s="7" t="s">
         <v>106</v>
@@ -3458,7 +3457,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="116"/>
+      <c r="C11" s="121"/>
       <c r="D11" s="15"/>
       <c r="E11" s="7" t="s">
         <v>107</v>
@@ -3487,7 +3486,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="116"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="15"/>
       <c r="E12" s="7" t="s">
         <v>108</v>
@@ -3516,7 +3515,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="116"/>
+      <c r="C13" s="121"/>
       <c r="D13" s="33"/>
       <c r="E13" s="7" t="s">
         <v>109</v>
@@ -3545,7 +3544,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C14" s="116"/>
+      <c r="C14" s="121"/>
       <c r="D14" s="33"/>
       <c r="E14" s="7" t="s">
         <v>110</v>
@@ -3574,7 +3573,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C15" s="116"/>
+      <c r="C15" s="121"/>
       <c r="D15" s="33"/>
       <c r="E15" s="7" t="s">
         <v>104</v>
@@ -3603,7 +3602,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C16" s="117"/>
+      <c r="C16" s="122"/>
       <c r="D16" s="16"/>
       <c r="E16" s="7" t="s">
         <v>112</v>
@@ -3642,98 +3641,98 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="115"/>
-      <c r="L18" s="115"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="103"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="114"/>
       <c r="G20" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="100" t="s">
+      <c r="H20" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="101"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="100" t="s">
+      <c r="I20" s="123"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="101"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="103"/>
+      <c r="N20" s="123"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="114"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="123" t="s">
+      <c r="B21" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="104" t="s">
+      <c r="E21" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="105" t="s">
+      <c r="F21" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="114" t="s">
+      <c r="G21" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="110" t="s">
+      <c r="H21" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="111"/>
-      <c r="J21" s="75" t="s">
+      <c r="I21" s="116"/>
+      <c r="J21" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="K21" s="75" t="s">
+      <c r="K21" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="L21" s="106" t="s">
+      <c r="L21" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="M21" s="108" t="s">
+      <c r="M21" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="104" t="s">
+      <c r="N21" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="O21" s="104" t="s">
+      <c r="O21" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="P21" s="105" t="s">
+      <c r="P21" s="111" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="123"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="112"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="107"/>
-      <c r="M22" s="109"/>
-      <c r="N22" s="104"/>
-      <c r="O22" s="104"/>
-      <c r="P22" s="105"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="124"/>
+      <c r="M22" s="126"/>
+      <c r="N22" s="110"/>
+      <c r="O22" s="110"/>
+      <c r="P22" s="111"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
@@ -3754,10 +3753,10 @@
       <c r="G23" s="27">
         <v>3</v>
       </c>
-      <c r="H23" s="121" t="s">
+      <c r="H23" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="I23" s="122"/>
+      <c r="I23" s="107"/>
       <c r="J23" s="2">
         <v>5</v>
       </c>
@@ -3782,6 +3781,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C6:C16"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="F4:I4"/>
@@ -3790,26 +3809,6 @@
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C6:C16"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3818,18 +3817,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3971,18 +3970,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5992EABF-6D8D-4DC8-AD0E-FD37EDF056C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7D9D9E-6447-4BB8-AD3E-F6023F68C701}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7D9D9E-6447-4BB8-AD3E-F6023F68C701}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5992EABF-6D8D-4DC8-AD0E-FD37EDF056C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>